<commit_message>
Update Excel lab 2023-Assignment 4- Refrence function & What if analysis.xlsx
</commit_message>
<xml_diff>
--- a/assignments/Excel lab 2023-Assignment 4- Refrence function & What if analysis.xlsx
+++ b/assignments/Excel lab 2023-Assignment 4- Refrence function & What if analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Humna\Documents\GitHub\mis201\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D95E3A-D930-4697-BF8F-8596FD3D217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A5DB9-58F1-4BE6-A47D-467E6C8E2586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D30AC0E5-DEDD-F84A-80E0-6A7288FD1CD5}"/>
   </bookViews>
@@ -2115,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C88F94D-0F29-2B46-A698-24AF8CB92F66}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2245,8 +2245,7 @@
         <v>104</v>
       </c>
       <c r="B17" s="19">
-        <f>55000-AVERAGE(B6:B16)</f>
-        <v>2907.8181818181838</v>
+        <v>86986</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -2254,11 +2253,15 @@
         <v>103</v>
       </c>
       <c r="B18" s="18">
-        <f>AVERAGE(B6:B16)</f>
-        <v>52092.181818181816</v>
+        <v>55000</v>
       </c>
     </row>
   </sheetData>
+  <scenarios current="0">
+    <scenario name="change aver" locked="1" count="1" user="Humna" comment="Created by Humna on 10/11/2023">
+      <inputCells r="B17" val="2907.81818181818"/>
+    </scenario>
+  </scenarios>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>